<commit_message>
Lab 4 Buggy Code
Problems with moveAway.
PID tuned
</commit_message>
<xml_diff>
--- a/Labs/Lab04/Light Sensor Measurements.xlsx
+++ b/Labs/Lab04/Light Sensor Measurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CONDITIONS</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Right Photoresistor (V)</t>
+  </si>
+  <si>
+    <t>D219 Location</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -233,6 +236,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +558,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,8 +568,11 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -570,8 +582,14 @@
       <c r="C2" s="7">
         <v>4.32</v>
       </c>
+      <c r="D2" s="12">
+        <v>4.12</v>
+      </c>
+      <c r="E2">
+        <v>4.18</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -581,8 +599,9 @@
       <c r="C3" s="7">
         <v>3.25</v>
       </c>
+      <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -592,8 +611,9 @@
       <c r="C4" s="7">
         <v>2.1</v>
       </c>
+      <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -603,8 +623,9 @@
       <c r="C5" s="10">
         <v>4.71</v>
       </c>
+      <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Lab 4 Buggy Code"
This reverts commit 8fae58a936e165186baae0615c8e262044adc59d.
</commit_message>
<xml_diff>
--- a/Labs/Lab04/Light Sensor Measurements.xlsx
+++ b/Labs/Lab04/Light Sensor Measurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CONDITIONS</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Right Photoresistor (V)</t>
-  </si>
-  <si>
-    <t>D219 Location</t>
   </si>
 </sst>
 </file>
@@ -210,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,12 +233,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -545,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +549,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -568,11 +559,8 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -582,14 +570,8 @@
       <c r="C2" s="7">
         <v>4.32</v>
       </c>
-      <c r="D2" s="12">
-        <v>4.12</v>
-      </c>
-      <c r="E2">
-        <v>4.18</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -599,9 +581,8 @@
       <c r="C3" s="7">
         <v>3.25</v>
       </c>
-      <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -611,9 +592,8 @@
       <c r="C4" s="7">
         <v>2.1</v>
       </c>
-      <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -623,9 +603,8 @@
       <c r="C5" s="10">
         <v>4.71</v>
       </c>
-      <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Lab 4 Buggy Code""
This reverts commit c9c27135b821b06aadb6aa66f5c2712950c98df0.
</commit_message>
<xml_diff>
--- a/Labs/Lab04/Light Sensor Measurements.xlsx
+++ b/Labs/Lab04/Light Sensor Measurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CONDITIONS</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Right Photoresistor (V)</t>
+  </si>
+  <si>
+    <t>D219 Location</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -233,6 +236,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +558,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,8 +568,11 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -570,8 +582,14 @@
       <c r="C2" s="7">
         <v>4.32</v>
       </c>
+      <c r="D2" s="12">
+        <v>4.12</v>
+      </c>
+      <c r="E2">
+        <v>4.18</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -581,8 +599,9 @@
       <c r="C3" s="7">
         <v>3.25</v>
       </c>
+      <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -592,8 +611,9 @@
       <c r="C4" s="7">
         <v>2.1</v>
       </c>
+      <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -603,8 +623,9 @@
       <c r="C5" s="10">
         <v>4.71</v>
       </c>
+      <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Lab 4 Buggy Code"""
This reverts commit 5692e0fbb0038b51a7243b6a04f750f48fc5844f.
</commit_message>
<xml_diff>
--- a/Labs/Lab04/Light Sensor Measurements.xlsx
+++ b/Labs/Lab04/Light Sensor Measurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CONDITIONS</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Right Photoresistor (V)</t>
-  </si>
-  <si>
-    <t>D219 Location</t>
   </si>
 </sst>
 </file>
@@ -210,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,12 +233,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -545,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +549,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -568,11 +559,8 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -582,14 +570,8 @@
       <c r="C2" s="7">
         <v>4.32</v>
       </c>
-      <c r="D2" s="12">
-        <v>4.12</v>
-      </c>
-      <c r="E2">
-        <v>4.18</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -599,9 +581,8 @@
       <c r="C3" s="7">
         <v>3.25</v>
       </c>
-      <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -611,9 +592,8 @@
       <c r="C4" s="7">
         <v>2.1</v>
       </c>
-      <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -623,9 +603,8 @@
       <c r="C5" s="10">
         <v>4.71</v>
       </c>
-      <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>